<commit_message>
- fexed measurement temperatures reported for `10.1016/j.intermet.2014.07.021` from incorrect range and unit
</commit_message>
<xml_diff>
--- a/HuiSun_HardnessData_Jan2022_AdamFix.xlsx
+++ b/HuiSun_HardnessData_Jan2022_AdamFix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-guest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D26D319-5964-4744-AD51-F83A45077D28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384F033E-A8A6-A541-983A-AF1000236E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1603,33 +1603,16 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1681,16 +1664,33 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -23099,8 +23099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="89" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F97" sqref="F97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -23136,21 +23136,21 @@
       <c r="B2" s="16" t="s">
         <v>235</v>
       </c>
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="53"/>
-      <c r="F2" s="48" t="s">
+      <c r="E2" s="52"/>
+      <c r="F2" s="47" t="s">
         <v>234</v>
       </c>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="49"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="48"/>
       <c r="O2" s="27"/>
     </row>
     <row r="3" spans="1:20" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -23160,17 +23160,17 @@
       <c r="B3" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="D3" s="54"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="51"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="50"/>
       <c r="O3" s="27"/>
     </row>
     <row r="4" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -23188,43 +23188,43 @@
       <c r="B5" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="64" t="s">
+      <c r="C5" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="45" t="s">
+      <c r="D5" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="45" t="s">
+      <c r="E5" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="45" t="s">
+      <c r="F5" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="45" t="s">
+      <c r="G5" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="46" t="s">
+      <c r="H5" s="71" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="45" t="s">
+      <c r="I5" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="J5" s="45" t="s">
+      <c r="J5" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="45" t="s">
+      <c r="K5" s="64" t="s">
         <v>46</v>
       </c>
-      <c r="L5" s="45" t="s">
+      <c r="L5" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="45" t="s">
+      <c r="M5" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="N5" s="45" t="s">
+      <c r="N5" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="O5" s="39" t="s">
+      <c r="O5" s="65" t="s">
         <v>50</v>
       </c>
     </row>
@@ -23235,19 +23235,19 @@
       <c r="B6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
-      <c r="O6" s="40"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="64"/>
+      <c r="J6" s="64"/>
+      <c r="K6" s="64"/>
+      <c r="L6" s="64"/>
+      <c r="M6" s="64"/>
+      <c r="N6" s="64"/>
+      <c r="O6" s="66"/>
     </row>
     <row r="7" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -23292,7 +23292,7 @@
       <c r="N7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O7" s="41"/>
+      <c r="O7" s="67"/>
       <c r="P7" s="33" t="s">
         <v>40</v>
       </c>
@@ -23305,35 +23305,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="59" t="s">
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="61"/>
-      <c r="K8" s="61"/>
-      <c r="L8" s="61"/>
-      <c r="M8" s="62" t="s">
+      <c r="G8" s="59"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="60"/>
+      <c r="K8" s="60"/>
+      <c r="L8" s="60"/>
+      <c r="M8" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="63"/>
+      <c r="N8" s="62"/>
       <c r="O8" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="P8" s="42" t="s">
+      <c r="P8" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="Q8" s="43"/>
-      <c r="R8" s="43"/>
-      <c r="S8" s="43"/>
-      <c r="T8" s="44"/>
+      <c r="Q8" s="69"/>
+      <c r="R8" s="69"/>
+      <c r="S8" s="69"/>
+      <c r="T8" s="70"/>
     </row>
     <row r="9" spans="1:20" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -23426,7 +23426,7 @@
       <c r="M10" t="s">
         <v>205</v>
       </c>
-      <c r="N10" s="69" t="s">
+      <c r="N10" s="43" t="s">
         <v>206</v>
       </c>
       <c r="O10" s="21"/>
@@ -23462,7 +23462,7 @@
       <c r="M11" t="s">
         <v>207</v>
       </c>
-      <c r="N11" s="69" t="s">
+      <c r="N11" s="43" t="s">
         <v>206</v>
       </c>
       <c r="O11" s="21"/>
@@ -23471,7 +23471,7 @@
       <c r="A12">
         <v>3</v>
       </c>
-      <c r="B12" s="65" t="s">
+      <c r="B12" s="39" t="s">
         <v>201</v>
       </c>
       <c r="C12" t="s">
@@ -23498,7 +23498,7 @@
       <c r="M12" t="s">
         <v>207</v>
       </c>
-      <c r="N12" s="69" t="s">
+      <c r="N12" s="43" t="s">
         <v>208</v>
       </c>
       <c r="O12" s="22"/>
@@ -23507,7 +23507,7 @@
       <c r="A13">
         <v>4</v>
       </c>
-      <c r="B13" s="65" t="s">
+      <c r="B13" s="39" t="s">
         <v>200</v>
       </c>
       <c r="C13" t="s">
@@ -23534,7 +23534,7 @@
       <c r="M13" t="s">
         <v>207</v>
       </c>
-      <c r="N13" s="69" t="s">
+      <c r="N13" s="43" t="s">
         <v>206</v>
       </c>
       <c r="O13" s="21"/>
@@ -23543,7 +23543,7 @@
       <c r="A14">
         <v>5</v>
       </c>
-      <c r="B14" s="65" t="s">
+      <c r="B14" s="39" t="s">
         <v>199</v>
       </c>
       <c r="C14" t="s">
@@ -23570,7 +23570,7 @@
       <c r="M14" t="s">
         <v>207</v>
       </c>
-      <c r="N14" s="69" t="s">
+      <c r="N14" s="43" t="s">
         <v>208</v>
       </c>
       <c r="O14" s="21"/>
@@ -23579,7 +23579,7 @@
       <c r="A15">
         <v>6</v>
       </c>
-      <c r="B15" s="65" t="s">
+      <c r="B15" s="39" t="s">
         <v>198</v>
       </c>
       <c r="C15" t="s">
@@ -23606,7 +23606,7 @@
       <c r="M15" t="s">
         <v>207</v>
       </c>
-      <c r="N15" s="69" t="s">
+      <c r="N15" s="43" t="s">
         <v>208</v>
       </c>
       <c r="O15" s="21"/>
@@ -23615,7 +23615,7 @@
       <c r="A16">
         <v>7</v>
       </c>
-      <c r="B16" s="65" t="s">
+      <c r="B16" s="39" t="s">
         <v>197</v>
       </c>
       <c r="C16" t="s">
@@ -23642,7 +23642,7 @@
       <c r="M16" t="s">
         <v>207</v>
       </c>
-      <c r="N16" s="69" t="s">
+      <c r="N16" s="43" t="s">
         <v>208</v>
       </c>
       <c r="O16" s="21"/>
@@ -23651,7 +23651,7 @@
       <c r="A17">
         <v>8</v>
       </c>
-      <c r="B17" s="65" t="s">
+      <c r="B17" s="39" t="s">
         <v>196</v>
       </c>
       <c r="C17" t="s">
@@ -23678,7 +23678,7 @@
       <c r="M17" t="s">
         <v>207</v>
       </c>
-      <c r="N17" s="69" t="s">
+      <c r="N17" s="43" t="s">
         <v>208</v>
       </c>
     </row>
@@ -23686,7 +23686,7 @@
       <c r="A18">
         <v>9</v>
       </c>
-      <c r="B18" s="65" t="s">
+      <c r="B18" s="39" t="s">
         <v>195</v>
       </c>
       <c r="C18" t="s">
@@ -23713,7 +23713,7 @@
       <c r="M18" t="s">
         <v>207</v>
       </c>
-      <c r="N18" s="69" t="s">
+      <c r="N18" s="43" t="s">
         <v>208</v>
       </c>
     </row>
@@ -23721,7 +23721,7 @@
       <c r="A19">
         <v>10</v>
       </c>
-      <c r="B19" s="65" t="s">
+      <c r="B19" s="39" t="s">
         <v>194</v>
       </c>
       <c r="C19" t="s">
@@ -23748,7 +23748,7 @@
       <c r="M19" t="s">
         <v>207</v>
       </c>
-      <c r="N19" s="69" t="s">
+      <c r="N19" s="43" t="s">
         <v>208</v>
       </c>
     </row>
@@ -23756,7 +23756,7 @@
       <c r="A20">
         <v>11</v>
       </c>
-      <c r="B20" s="65" t="s">
+      <c r="B20" s="39" t="s">
         <v>193</v>
       </c>
       <c r="C20" t="s">
@@ -23783,7 +23783,7 @@
       <c r="M20" t="s">
         <v>207</v>
       </c>
-      <c r="N20" s="69" t="s">
+      <c r="N20" s="43" t="s">
         <v>208</v>
       </c>
     </row>
@@ -23791,7 +23791,7 @@
       <c r="A21">
         <v>12</v>
       </c>
-      <c r="B21" s="65" t="s">
+      <c r="B21" s="39" t="s">
         <v>192</v>
       </c>
       <c r="C21" t="s">
@@ -23818,7 +23818,7 @@
       <c r="M21" t="s">
         <v>207</v>
       </c>
-      <c r="N21" s="69" t="s">
+      <c r="N21" s="43" t="s">
         <v>208</v>
       </c>
     </row>
@@ -23826,7 +23826,7 @@
       <c r="A22">
         <v>13</v>
       </c>
-      <c r="B22" s="65" t="s">
+      <c r="B22" s="39" t="s">
         <v>191</v>
       </c>
       <c r="C22" t="s">
@@ -23853,7 +23853,7 @@
       <c r="M22" t="s">
         <v>207</v>
       </c>
-      <c r="N22" s="69" t="s">
+      <c r="N22" s="43" t="s">
         <v>208</v>
       </c>
     </row>
@@ -23861,7 +23861,7 @@
       <c r="A23">
         <v>14</v>
       </c>
-      <c r="B23" s="65" t="s">
+      <c r="B23" s="39" t="s">
         <v>190</v>
       </c>
       <c r="C23" t="s">
@@ -23888,7 +23888,7 @@
       <c r="M23" t="s">
         <v>207</v>
       </c>
-      <c r="N23" s="69" t="s">
+      <c r="N23" s="43" t="s">
         <v>208</v>
       </c>
     </row>
@@ -23896,7 +23896,7 @@
       <c r="A24">
         <v>15</v>
       </c>
-      <c r="B24" s="65" t="s">
+      <c r="B24" s="39" t="s">
         <v>189</v>
       </c>
       <c r="C24" t="s">
@@ -23923,7 +23923,7 @@
       <c r="M24" t="s">
         <v>207</v>
       </c>
-      <c r="N24" s="69" t="s">
+      <c r="N24" s="43" t="s">
         <v>208</v>
       </c>
     </row>
@@ -23931,7 +23931,7 @@
       <c r="A25">
         <v>16</v>
       </c>
-      <c r="B25" s="65" t="s">
+      <c r="B25" s="39" t="s">
         <v>188</v>
       </c>
       <c r="C25" t="s">
@@ -23958,7 +23958,7 @@
       <c r="M25" t="s">
         <v>207</v>
       </c>
-      <c r="N25" s="69" t="s">
+      <c r="N25" s="43" t="s">
         <v>208</v>
       </c>
     </row>
@@ -23966,7 +23966,7 @@
       <c r="A26">
         <v>17</v>
       </c>
-      <c r="B26" s="65" t="s">
+      <c r="B26" s="39" t="s">
         <v>187</v>
       </c>
       <c r="C26" t="s">
@@ -23993,7 +23993,7 @@
       <c r="M26" t="s">
         <v>207</v>
       </c>
-      <c r="N26" s="69" t="s">
+      <c r="N26" s="43" t="s">
         <v>208</v>
       </c>
     </row>
@@ -24001,7 +24001,7 @@
       <c r="A27">
         <v>18</v>
       </c>
-      <c r="B27" s="65" t="s">
+      <c r="B27" s="39" t="s">
         <v>186</v>
       </c>
       <c r="C27" t="s">
@@ -24028,7 +24028,7 @@
       <c r="M27" t="s">
         <v>207</v>
       </c>
-      <c r="N27" s="69" t="s">
+      <c r="N27" s="43" t="s">
         <v>208</v>
       </c>
     </row>
@@ -24036,7 +24036,7 @@
       <c r="A28">
         <v>19</v>
       </c>
-      <c r="B28" s="65" t="s">
+      <c r="B28" s="39" t="s">
         <v>185</v>
       </c>
       <c r="C28" t="s">
@@ -24063,7 +24063,7 @@
       <c r="M28" t="s">
         <v>207</v>
       </c>
-      <c r="N28" s="69" t="s">
+      <c r="N28" s="43" t="s">
         <v>208</v>
       </c>
     </row>
@@ -24071,7 +24071,7 @@
       <c r="A29">
         <v>20</v>
       </c>
-      <c r="B29" s="65" t="s">
+      <c r="B29" s="39" t="s">
         <v>183</v>
       </c>
       <c r="C29" t="s">
@@ -24098,7 +24098,7 @@
       <c r="M29" t="s">
         <v>207</v>
       </c>
-      <c r="N29" s="69" t="s">
+      <c r="N29" s="43" t="s">
         <v>208</v>
       </c>
     </row>
@@ -24106,7 +24106,7 @@
       <c r="A30">
         <v>21</v>
       </c>
-      <c r="B30" s="65" t="s">
+      <c r="B30" s="39" t="s">
         <v>182</v>
       </c>
       <c r="C30" t="s">
@@ -24133,7 +24133,7 @@
       <c r="M30" t="s">
         <v>207</v>
       </c>
-      <c r="N30" s="69" t="s">
+      <c r="N30" s="43" t="s">
         <v>208</v>
       </c>
     </row>
@@ -24141,7 +24141,7 @@
       <c r="A31">
         <v>22</v>
       </c>
-      <c r="B31" s="65" t="s">
+      <c r="B31" s="39" t="s">
         <v>181</v>
       </c>
       <c r="C31" t="s">
@@ -24168,7 +24168,7 @@
       <c r="M31" t="s">
         <v>207</v>
       </c>
-      <c r="N31" s="69" t="s">
+      <c r="N31" s="43" t="s">
         <v>208</v>
       </c>
     </row>
@@ -24176,7 +24176,7 @@
       <c r="A32">
         <v>23</v>
       </c>
-      <c r="B32" s="65" t="s">
+      <c r="B32" s="39" t="s">
         <v>179</v>
       </c>
       <c r="C32" t="s">
@@ -24203,7 +24203,7 @@
       <c r="M32" t="s">
         <v>207</v>
       </c>
-      <c r="N32" s="69" t="s">
+      <c r="N32" s="43" t="s">
         <v>208</v>
       </c>
     </row>
@@ -24211,7 +24211,7 @@
       <c r="A33">
         <v>24</v>
       </c>
-      <c r="B33" s="65" t="s">
+      <c r="B33" s="39" t="s">
         <v>178</v>
       </c>
       <c r="C33" t="s">
@@ -24238,7 +24238,7 @@
       <c r="M33" t="s">
         <v>207</v>
       </c>
-      <c r="N33" s="69" t="s">
+      <c r="N33" s="43" t="s">
         <v>208</v>
       </c>
     </row>
@@ -24246,7 +24246,7 @@
       <c r="A34">
         <v>25</v>
       </c>
-      <c r="B34" s="65" t="s">
+      <c r="B34" s="39" t="s">
         <v>177</v>
       </c>
       <c r="C34" t="s">
@@ -24273,7 +24273,7 @@
       <c r="M34" t="s">
         <v>207</v>
       </c>
-      <c r="N34" s="69" t="s">
+      <c r="N34" s="43" t="s">
         <v>208</v>
       </c>
     </row>
@@ -24281,7 +24281,7 @@
       <c r="A35">
         <v>26</v>
       </c>
-      <c r="B35" s="65" t="s">
+      <c r="B35" s="39" t="s">
         <v>176</v>
       </c>
       <c r="C35" t="s">
@@ -24308,7 +24308,7 @@
       <c r="M35" t="s">
         <v>207</v>
       </c>
-      <c r="N35" s="69" t="s">
+      <c r="N35" s="43" t="s">
         <v>208</v>
       </c>
     </row>
@@ -24316,7 +24316,7 @@
       <c r="A36">
         <v>27</v>
       </c>
-      <c r="B36" s="65" t="s">
+      <c r="B36" s="39" t="s">
         <v>175</v>
       </c>
       <c r="C36" t="s">
@@ -24343,7 +24343,7 @@
       <c r="M36" t="s">
         <v>207</v>
       </c>
-      <c r="N36" s="69" t="s">
+      <c r="N36" s="43" t="s">
         <v>208</v>
       </c>
     </row>
@@ -24351,7 +24351,7 @@
       <c r="A37">
         <v>28</v>
       </c>
-      <c r="B37" s="65" t="s">
+      <c r="B37" s="39" t="s">
         <v>174</v>
       </c>
       <c r="C37" t="s">
@@ -24378,7 +24378,7 @@
       <c r="M37" t="s">
         <v>207</v>
       </c>
-      <c r="N37" s="69" t="s">
+      <c r="N37" s="43" t="s">
         <v>208</v>
       </c>
     </row>
@@ -24386,7 +24386,7 @@
       <c r="A38">
         <v>29</v>
       </c>
-      <c r="B38" s="65" t="s">
+      <c r="B38" s="39" t="s">
         <v>172</v>
       </c>
       <c r="C38" t="s">
@@ -24410,7 +24410,7 @@
       <c r="M38" t="s">
         <v>207</v>
       </c>
-      <c r="N38" s="70" t="s">
+      <c r="N38" s="44" t="s">
         <v>209</v>
       </c>
     </row>
@@ -24418,7 +24418,7 @@
       <c r="A39">
         <v>30</v>
       </c>
-      <c r="B39" s="65" t="s">
+      <c r="B39" s="39" t="s">
         <v>171</v>
       </c>
       <c r="C39" t="s">
@@ -24442,7 +24442,7 @@
       <c r="M39" t="s">
         <v>207</v>
       </c>
-      <c r="N39" s="70" t="s">
+      <c r="N39" s="44" t="s">
         <v>209</v>
       </c>
     </row>
@@ -24450,7 +24450,7 @@
       <c r="A40">
         <v>31</v>
       </c>
-      <c r="B40" s="65" t="s">
+      <c r="B40" s="39" t="s">
         <v>170</v>
       </c>
       <c r="C40" t="s">
@@ -24474,7 +24474,7 @@
       <c r="M40" t="s">
         <v>207</v>
       </c>
-      <c r="N40" s="70" t="s">
+      <c r="N40" s="44" t="s">
         <v>209</v>
       </c>
     </row>
@@ -24482,7 +24482,7 @@
       <c r="A41">
         <v>32</v>
       </c>
-      <c r="B41" s="65" t="s">
+      <c r="B41" s="39" t="s">
         <v>169</v>
       </c>
       <c r="C41" t="s">
@@ -24506,7 +24506,7 @@
       <c r="M41" t="s">
         <v>207</v>
       </c>
-      <c r="N41" s="70" t="s">
+      <c r="N41" s="44" t="s">
         <v>209</v>
       </c>
     </row>
@@ -24514,7 +24514,7 @@
       <c r="A42">
         <v>33</v>
       </c>
-      <c r="B42" s="65" t="s">
+      <c r="B42" s="39" t="s">
         <v>83</v>
       </c>
       <c r="C42" t="s">
@@ -24538,7 +24538,7 @@
       <c r="M42" t="s">
         <v>207</v>
       </c>
-      <c r="N42" s="70" t="s">
+      <c r="N42" s="44" t="s">
         <v>209</v>
       </c>
     </row>
@@ -24546,7 +24546,7 @@
       <c r="A43">
         <v>34</v>
       </c>
-      <c r="B43" s="65" t="s">
+      <c r="B43" s="39" t="s">
         <v>167</v>
       </c>
       <c r="C43" t="s">
@@ -24570,7 +24570,7 @@
       <c r="M43" t="s">
         <v>205</v>
       </c>
-      <c r="N43" s="71" t="s">
+      <c r="N43" s="45" t="s">
         <v>210</v>
       </c>
     </row>
@@ -24578,7 +24578,7 @@
       <c r="A44">
         <v>35</v>
       </c>
-      <c r="B44" s="65" t="s">
+      <c r="B44" s="39" t="s">
         <v>168</v>
       </c>
       <c r="C44" t="s">
@@ -24602,7 +24602,7 @@
       <c r="M44" t="s">
         <v>211</v>
       </c>
-      <c r="N44" s="71" t="s">
+      <c r="N44" s="45" t="s">
         <v>210</v>
       </c>
     </row>
@@ -24610,7 +24610,7 @@
       <c r="A45">
         <v>36</v>
       </c>
-      <c r="B45" s="65" t="s">
+      <c r="B45" s="39" t="s">
         <v>167</v>
       </c>
       <c r="C45" t="s">
@@ -24634,7 +24634,7 @@
       <c r="M45" t="s">
         <v>211</v>
       </c>
-      <c r="N45" s="71" t="s">
+      <c r="N45" s="45" t="s">
         <v>210</v>
       </c>
     </row>
@@ -24642,7 +24642,7 @@
       <c r="A46">
         <v>37</v>
       </c>
-      <c r="B46" s="65" t="s">
+      <c r="B46" s="39" t="s">
         <v>161</v>
       </c>
       <c r="C46" t="s">
@@ -24666,7 +24666,7 @@
       <c r="M46" t="s">
         <v>211</v>
       </c>
-      <c r="N46" s="71" t="s">
+      <c r="N46" s="45" t="s">
         <v>210</v>
       </c>
     </row>
@@ -24674,7 +24674,7 @@
       <c r="A47">
         <v>38</v>
       </c>
-      <c r="B47" s="65" t="s">
+      <c r="B47" s="39" t="s">
         <v>166</v>
       </c>
       <c r="C47" t="s">
@@ -24698,7 +24698,7 @@
       <c r="M47" t="s">
         <v>211</v>
       </c>
-      <c r="N47" s="71" t="s">
+      <c r="N47" s="45" t="s">
         <v>210</v>
       </c>
     </row>
@@ -24706,7 +24706,7 @@
       <c r="A48">
         <v>39</v>
       </c>
-      <c r="B48" s="65" t="s">
+      <c r="B48" s="39" t="s">
         <v>164</v>
       </c>
       <c r="C48" t="s">
@@ -24730,7 +24730,7 @@
       <c r="M48" t="s">
         <v>211</v>
       </c>
-      <c r="N48" s="71" t="s">
+      <c r="N48" s="45" t="s">
         <v>210</v>
       </c>
     </row>
@@ -24738,7 +24738,7 @@
       <c r="A49">
         <v>40</v>
       </c>
-      <c r="B49" s="65" t="s">
+      <c r="B49" s="39" t="s">
         <v>163</v>
       </c>
       <c r="C49" t="s">
@@ -24762,7 +24762,7 @@
       <c r="M49" t="s">
         <v>211</v>
       </c>
-      <c r="N49" s="71" t="s">
+      <c r="N49" s="45" t="s">
         <v>210</v>
       </c>
     </row>
@@ -24770,7 +24770,7 @@
       <c r="A50">
         <v>41</v>
       </c>
-      <c r="B50" s="65" t="s">
+      <c r="B50" s="39" t="s">
         <v>162</v>
       </c>
       <c r="C50" t="s">
@@ -24794,7 +24794,7 @@
       <c r="M50" t="s">
         <v>211</v>
       </c>
-      <c r="N50" s="71" t="s">
+      <c r="N50" s="45" t="s">
         <v>210</v>
       </c>
     </row>
@@ -24802,7 +24802,7 @@
       <c r="A51">
         <v>42</v>
       </c>
-      <c r="B51" s="65" t="s">
+      <c r="B51" s="39" t="s">
         <v>161</v>
       </c>
       <c r="C51" t="s">
@@ -24829,7 +24829,7 @@
       <c r="M51" t="s">
         <v>212</v>
       </c>
-      <c r="N51" s="69" t="s">
+      <c r="N51" s="43" t="s">
         <v>213</v>
       </c>
     </row>
@@ -24837,7 +24837,7 @@
       <c r="A52">
         <v>43</v>
       </c>
-      <c r="B52" s="65" t="s">
+      <c r="B52" s="39" t="s">
         <v>159</v>
       </c>
       <c r="C52" t="s">
@@ -24869,7 +24869,7 @@
       <c r="A53">
         <v>44</v>
       </c>
-      <c r="B53" s="65" t="s">
+      <c r="B53" s="39" t="s">
         <v>158</v>
       </c>
       <c r="C53" t="s">
@@ -24901,7 +24901,7 @@
       <c r="A54">
         <v>45</v>
       </c>
-      <c r="B54" s="65" t="s">
+      <c r="B54" s="39" t="s">
         <v>157</v>
       </c>
       <c r="C54" t="s">
@@ -24933,7 +24933,7 @@
       <c r="A55">
         <v>46</v>
       </c>
-      <c r="B55" s="65" t="s">
+      <c r="B55" s="39" t="s">
         <v>156</v>
       </c>
       <c r="C55" t="s">
@@ -24965,7 +24965,7 @@
       <c r="A56">
         <v>47</v>
       </c>
-      <c r="B56" s="65" t="s">
+      <c r="B56" s="39" t="s">
         <v>155</v>
       </c>
       <c r="C56" t="s">
@@ -24997,7 +24997,7 @@
       <c r="A57">
         <v>48</v>
       </c>
-      <c r="B57" s="65" t="s">
+      <c r="B57" s="39" t="s">
         <v>154</v>
       </c>
       <c r="C57" t="s">
@@ -25029,7 +25029,7 @@
       <c r="A58">
         <v>49</v>
       </c>
-      <c r="B58" s="65" t="s">
+      <c r="B58" s="39" t="s">
         <v>153</v>
       </c>
       <c r="C58" t="s">
@@ -25061,7 +25061,7 @@
       <c r="A59">
         <v>50</v>
       </c>
-      <c r="B59" s="65" t="s">
+      <c r="B59" s="39" t="s">
         <v>151</v>
       </c>
       <c r="C59" t="s">
@@ -25077,7 +25077,7 @@
       <c r="J59" s="34"/>
       <c r="K59" s="34"/>
       <c r="L59" s="21"/>
-      <c r="N59" s="71" t="s">
+      <c r="N59" s="45" t="s">
         <v>215</v>
       </c>
     </row>
@@ -25115,7 +25115,7 @@
       <c r="M60" t="s">
         <v>216</v>
       </c>
-      <c r="N60" s="71" t="s">
+      <c r="N60" s="45" t="s">
         <v>215</v>
       </c>
     </row>
@@ -25123,7 +25123,7 @@
       <c r="A61">
         <v>52</v>
       </c>
-      <c r="B61" s="65" t="s">
+      <c r="B61" s="39" t="s">
         <v>147</v>
       </c>
       <c r="C61" t="s">
@@ -25150,7 +25150,7 @@
       <c r="M61" t="s">
         <v>217</v>
       </c>
-      <c r="N61" s="71" t="s">
+      <c r="N61" s="45" t="s">
         <v>218</v>
       </c>
     </row>
@@ -25158,7 +25158,7 @@
       <c r="A62">
         <v>53</v>
       </c>
-      <c r="B62" s="65" t="s">
+      <c r="B62" s="39" t="s">
         <v>147</v>
       </c>
       <c r="C62" t="s">
@@ -25185,7 +25185,7 @@
       <c r="M62" t="s">
         <v>217</v>
       </c>
-      <c r="N62" s="71" t="s">
+      <c r="N62" s="45" t="s">
         <v>218</v>
       </c>
     </row>
@@ -25193,10 +25193,10 @@
       <c r="A63">
         <v>54</v>
       </c>
-      <c r="B63" s="65" t="s">
+      <c r="B63" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="C63" s="65" t="s">
+      <c r="C63" s="39" t="s">
         <v>115</v>
       </c>
       <c r="F63" t="s">
@@ -25217,7 +25217,7 @@
       <c r="M63" t="s">
         <v>211</v>
       </c>
-      <c r="N63" s="71" t="s">
+      <c r="N63" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -25225,10 +25225,10 @@
       <c r="A64">
         <v>55</v>
       </c>
-      <c r="B64" s="65" t="s">
+      <c r="B64" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="C64" s="65" t="s">
+      <c r="C64" s="39" t="s">
         <v>115</v>
       </c>
       <c r="F64" t="s">
@@ -25249,7 +25249,7 @@
       <c r="M64" t="s">
         <v>211</v>
       </c>
-      <c r="N64" s="71" t="s">
+      <c r="N64" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -25257,10 +25257,10 @@
       <c r="A65">
         <v>56</v>
       </c>
-      <c r="B65" s="65" t="s">
+      <c r="B65" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="C65" s="65" t="s">
+      <c r="C65" s="39" t="s">
         <v>115</v>
       </c>
       <c r="F65" t="s">
@@ -25281,7 +25281,7 @@
       <c r="M65" t="s">
         <v>211</v>
       </c>
-      <c r="N65" s="71" t="s">
+      <c r="N65" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -25289,10 +25289,10 @@
       <c r="A66">
         <v>57</v>
       </c>
-      <c r="B66" s="65" t="s">
+      <c r="B66" s="39" t="s">
         <v>143</v>
       </c>
-      <c r="C66" s="65" t="s">
+      <c r="C66" s="39" t="s">
         <v>66</v>
       </c>
       <c r="F66" t="s">
@@ -25313,7 +25313,7 @@
       <c r="M66" t="s">
         <v>211</v>
       </c>
-      <c r="N66" s="71" t="s">
+      <c r="N66" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -25321,10 +25321,10 @@
       <c r="A67">
         <v>58</v>
       </c>
-      <c r="B67" s="65" t="s">
+      <c r="B67" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="C67" s="65" t="s">
+      <c r="C67" s="39" t="s">
         <v>66</v>
       </c>
       <c r="F67" t="s">
@@ -25345,7 +25345,7 @@
       <c r="M67" t="s">
         <v>211</v>
       </c>
-      <c r="N67" s="71" t="s">
+      <c r="N67" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -25353,10 +25353,10 @@
       <c r="A68">
         <v>59</v>
       </c>
-      <c r="B68" s="65" t="s">
+      <c r="B68" s="39" t="s">
         <v>141</v>
       </c>
-      <c r="C68" s="65" t="s">
+      <c r="C68" s="39" t="s">
         <v>115</v>
       </c>
       <c r="F68" t="s">
@@ -25377,7 +25377,7 @@
       <c r="M68" t="s">
         <v>211</v>
       </c>
-      <c r="N68" s="71" t="s">
+      <c r="N68" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -25385,10 +25385,10 @@
       <c r="A69">
         <v>60</v>
       </c>
-      <c r="B69" s="65" t="s">
+      <c r="B69" s="39" t="s">
         <v>140</v>
       </c>
-      <c r="C69" s="65" t="s">
+      <c r="C69" s="39" t="s">
         <v>115</v>
       </c>
       <c r="F69" t="s">
@@ -25409,7 +25409,7 @@
       <c r="M69" t="s">
         <v>211</v>
       </c>
-      <c r="N69" s="71" t="s">
+      <c r="N69" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -25417,10 +25417,10 @@
       <c r="A70">
         <v>61</v>
       </c>
-      <c r="B70" s="65" t="s">
+      <c r="B70" s="39" t="s">
         <v>139</v>
       </c>
-      <c r="C70" s="65" t="s">
+      <c r="C70" s="39" t="s">
         <v>115</v>
       </c>
       <c r="F70" t="s">
@@ -25441,7 +25441,7 @@
       <c r="M70" t="s">
         <v>211</v>
       </c>
-      <c r="N70" s="71" t="s">
+      <c r="N70" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -25449,10 +25449,10 @@
       <c r="A71">
         <v>62</v>
       </c>
-      <c r="B71" s="65" t="s">
+      <c r="B71" s="39" t="s">
         <v>138</v>
       </c>
-      <c r="C71" s="65" t="s">
+      <c r="C71" s="39" t="s">
         <v>115</v>
       </c>
       <c r="F71" t="s">
@@ -25473,7 +25473,7 @@
       <c r="M71" t="s">
         <v>211</v>
       </c>
-      <c r="N71" s="71" t="s">
+      <c r="N71" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -25481,10 +25481,10 @@
       <c r="A72">
         <v>63</v>
       </c>
-      <c r="B72" s="65" t="s">
+      <c r="B72" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="C72" s="65" t="s">
+      <c r="C72" s="39" t="s">
         <v>115</v>
       </c>
       <c r="F72" t="s">
@@ -25505,7 +25505,7 @@
       <c r="M72" t="s">
         <v>211</v>
       </c>
-      <c r="N72" s="71" t="s">
+      <c r="N72" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -25513,10 +25513,10 @@
       <c r="A73">
         <v>64</v>
       </c>
-      <c r="B73" s="65" t="s">
+      <c r="B73" s="39" t="s">
         <v>136</v>
       </c>
-      <c r="C73" s="65" t="s">
+      <c r="C73" s="39" t="s">
         <v>115</v>
       </c>
       <c r="F73" t="s">
@@ -25537,7 +25537,7 @@
       <c r="M73" t="s">
         <v>211</v>
       </c>
-      <c r="N73" s="71" t="s">
+      <c r="N73" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -25545,10 +25545,10 @@
       <c r="A74">
         <v>65</v>
       </c>
-      <c r="B74" s="65" t="s">
+      <c r="B74" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="C74" s="65" t="s">
+      <c r="C74" s="39" t="s">
         <v>66</v>
       </c>
       <c r="F74" t="s">
@@ -25569,7 +25569,7 @@
       <c r="M74" t="s">
         <v>211</v>
       </c>
-      <c r="N74" s="71" t="s">
+      <c r="N74" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -25577,10 +25577,10 @@
       <c r="A75">
         <v>66</v>
       </c>
-      <c r="B75" s="65" t="s">
+      <c r="B75" s="39" t="s">
         <v>134</v>
       </c>
-      <c r="C75" s="65" t="s">
+      <c r="C75" s="39" t="s">
         <v>66</v>
       </c>
       <c r="F75" t="s">
@@ -25601,7 +25601,7 @@
       <c r="M75" t="s">
         <v>211</v>
       </c>
-      <c r="N75" s="71" t="s">
+      <c r="N75" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -25609,10 +25609,10 @@
       <c r="A76">
         <v>67</v>
       </c>
-      <c r="B76" s="65" t="s">
+      <c r="B76" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="C76" s="65" t="s">
+      <c r="C76" s="39" t="s">
         <v>66</v>
       </c>
       <c r="F76" t="s">
@@ -25633,7 +25633,7 @@
       <c r="M76" t="s">
         <v>211</v>
       </c>
-      <c r="N76" s="71" t="s">
+      <c r="N76" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -25641,10 +25641,10 @@
       <c r="A77">
         <v>68</v>
       </c>
-      <c r="B77" s="65" t="s">
+      <c r="B77" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="C77" s="65" t="s">
+      <c r="C77" s="39" t="s">
         <v>66</v>
       </c>
       <c r="F77" t="s">
@@ -25665,7 +25665,7 @@
       <c r="M77" t="s">
         <v>211</v>
       </c>
-      <c r="N77" s="71" t="s">
+      <c r="N77" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -25673,10 +25673,10 @@
       <c r="A78">
         <v>69</v>
       </c>
-      <c r="B78" s="65" t="s">
+      <c r="B78" s="39" t="s">
         <v>131</v>
       </c>
-      <c r="C78" s="65" t="s">
+      <c r="C78" s="39" t="s">
         <v>66</v>
       </c>
       <c r="F78" t="s">
@@ -25697,7 +25697,7 @@
       <c r="M78" t="s">
         <v>211</v>
       </c>
-      <c r="N78" s="71" t="s">
+      <c r="N78" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -25705,10 +25705,10 @@
       <c r="A79">
         <v>70</v>
       </c>
-      <c r="B79" s="65" t="s">
+      <c r="B79" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="C79" s="65" t="s">
+      <c r="C79" s="39" t="s">
         <v>115</v>
       </c>
       <c r="F79" t="s">
@@ -25729,7 +25729,7 @@
       <c r="M79" t="s">
         <v>211</v>
       </c>
-      <c r="N79" s="71" t="s">
+      <c r="N79" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -25737,10 +25737,10 @@
       <c r="A80">
         <v>71</v>
       </c>
-      <c r="B80" s="65" t="s">
+      <c r="B80" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="C80" s="65" t="s">
+      <c r="C80" s="39" t="s">
         <v>66</v>
       </c>
       <c r="F80" t="s">
@@ -25761,7 +25761,7 @@
       <c r="M80" t="s">
         <v>211</v>
       </c>
-      <c r="N80" s="71" t="s">
+      <c r="N80" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -25769,10 +25769,10 @@
       <c r="A81">
         <v>72</v>
       </c>
-      <c r="B81" s="65" t="s">
+      <c r="B81" s="39" t="s">
         <v>128</v>
       </c>
-      <c r="C81" s="65" t="s">
+      <c r="C81" s="39" t="s">
         <v>115</v>
       </c>
       <c r="F81" t="s">
@@ -25793,7 +25793,7 @@
       <c r="M81" t="s">
         <v>211</v>
       </c>
-      <c r="N81" s="71" t="s">
+      <c r="N81" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -25801,10 +25801,10 @@
       <c r="A82">
         <v>73</v>
       </c>
-      <c r="B82" s="65" t="s">
+      <c r="B82" s="39" t="s">
         <v>127</v>
       </c>
-      <c r="C82" s="65" t="s">
+      <c r="C82" s="39" t="s">
         <v>66</v>
       </c>
       <c r="F82" t="s">
@@ -25825,7 +25825,7 @@
       <c r="M82" t="s">
         <v>211</v>
       </c>
-      <c r="N82" s="71" t="s">
+      <c r="N82" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -25833,10 +25833,10 @@
       <c r="A83">
         <v>74</v>
       </c>
-      <c r="B83" s="65" t="s">
+      <c r="B83" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="C83" s="65" t="s">
+      <c r="C83" s="39" t="s">
         <v>115</v>
       </c>
       <c r="F83" t="s">
@@ -25857,7 +25857,7 @@
       <c r="M83" t="s">
         <v>211</v>
       </c>
-      <c r="N83" s="71" t="s">
+      <c r="N83" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -25865,10 +25865,10 @@
       <c r="A84">
         <v>75</v>
       </c>
-      <c r="B84" s="65" t="s">
+      <c r="B84" s="39" t="s">
         <v>125</v>
       </c>
-      <c r="C84" s="65" t="s">
+      <c r="C84" s="39" t="s">
         <v>115</v>
       </c>
       <c r="F84" t="s">
@@ -25889,7 +25889,7 @@
       <c r="M84" t="s">
         <v>211</v>
       </c>
-      <c r="N84" s="71" t="s">
+      <c r="N84" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -25897,10 +25897,10 @@
       <c r="A85">
         <v>76</v>
       </c>
-      <c r="B85" s="65" t="s">
+      <c r="B85" s="39" t="s">
         <v>124</v>
       </c>
-      <c r="C85" s="65" t="s">
+      <c r="C85" s="39" t="s">
         <v>115</v>
       </c>
       <c r="F85" t="s">
@@ -25921,7 +25921,7 @@
       <c r="M85" t="s">
         <v>211</v>
       </c>
-      <c r="N85" s="71" t="s">
+      <c r="N85" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -25929,10 +25929,10 @@
       <c r="A86">
         <v>77</v>
       </c>
-      <c r="B86" s="65" t="s">
+      <c r="B86" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="C86" s="65" t="s">
+      <c r="C86" s="39" t="s">
         <v>115</v>
       </c>
       <c r="F86" t="s">
@@ -25953,7 +25953,7 @@
       <c r="M86" t="s">
         <v>211</v>
       </c>
-      <c r="N86" s="71" t="s">
+      <c r="N86" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -25961,10 +25961,10 @@
       <c r="A87">
         <v>78</v>
       </c>
-      <c r="B87" s="65" t="s">
+      <c r="B87" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="C87" s="65" t="s">
+      <c r="C87" s="39" t="s">
         <v>115</v>
       </c>
       <c r="F87" t="s">
@@ -25985,7 +25985,7 @@
       <c r="M87" t="s">
         <v>211</v>
       </c>
-      <c r="N87" s="71" t="s">
+      <c r="N87" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -25993,10 +25993,10 @@
       <c r="A88">
         <v>79</v>
       </c>
-      <c r="B88" s="65" t="s">
+      <c r="B88" s="39" t="s">
         <v>121</v>
       </c>
-      <c r="C88" s="65" t="s">
+      <c r="C88" s="39" t="s">
         <v>66</v>
       </c>
       <c r="F88" t="s">
@@ -26017,7 +26017,7 @@
       <c r="M88" t="s">
         <v>211</v>
       </c>
-      <c r="N88" s="71" t="s">
+      <c r="N88" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -26025,10 +26025,10 @@
       <c r="A89">
         <v>80</v>
       </c>
-      <c r="B89" s="65" t="s">
+      <c r="B89" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="C89" s="65" t="s">
+      <c r="C89" s="39" t="s">
         <v>66</v>
       </c>
       <c r="F89" t="s">
@@ -26049,7 +26049,7 @@
       <c r="M89" t="s">
         <v>211</v>
       </c>
-      <c r="N89" s="71" t="s">
+      <c r="N89" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -26057,10 +26057,10 @@
       <c r="A90">
         <v>81</v>
       </c>
-      <c r="B90" s="65" t="s">
+      <c r="B90" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="C90" s="65" t="s">
+      <c r="C90" s="39" t="s">
         <v>66</v>
       </c>
       <c r="F90" t="s">
@@ -26081,7 +26081,7 @@
       <c r="M90" t="s">
         <v>211</v>
       </c>
-      <c r="N90" s="71" t="s">
+      <c r="N90" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -26089,10 +26089,10 @@
       <c r="A91">
         <v>82</v>
       </c>
-      <c r="B91" s="65" t="s">
+      <c r="B91" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="C91" s="65" t="s">
+      <c r="C91" s="39" t="s">
         <v>66</v>
       </c>
       <c r="F91" t="s">
@@ -26113,7 +26113,7 @@
       <c r="M91" t="s">
         <v>211</v>
       </c>
-      <c r="N91" s="71" t="s">
+      <c r="N91" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -26121,10 +26121,10 @@
       <c r="A92">
         <v>83</v>
       </c>
-      <c r="B92" s="65" t="s">
+      <c r="B92" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="C92" s="65" t="s">
+      <c r="C92" s="39" t="s">
         <v>66</v>
       </c>
       <c r="F92" t="s">
@@ -26145,7 +26145,7 @@
       <c r="M92" t="s">
         <v>211</v>
       </c>
-      <c r="N92" s="71" t="s">
+      <c r="N92" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -26153,10 +26153,10 @@
       <c r="A93">
         <v>84</v>
       </c>
-      <c r="B93" s="65" t="s">
+      <c r="B93" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="C93" s="65" t="s">
+      <c r="C93" s="39" t="s">
         <v>115</v>
       </c>
       <c r="F93" t="s">
@@ -26177,7 +26177,7 @@
       <c r="M93" t="s">
         <v>211</v>
       </c>
-      <c r="N93" s="71" t="s">
+      <c r="N93" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -26185,10 +26185,10 @@
       <c r="A94">
         <v>85</v>
       </c>
-      <c r="B94" s="65" t="s">
+      <c r="B94" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="C94" s="65" t="s">
+      <c r="C94" s="39" t="s">
         <v>66</v>
       </c>
       <c r="F94" t="s">
@@ -26209,7 +26209,7 @@
       <c r="M94" t="s">
         <v>211</v>
       </c>
-      <c r="N94" s="71" t="s">
+      <c r="N94" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -26217,10 +26217,10 @@
       <c r="A95">
         <v>86</v>
       </c>
-      <c r="B95" s="65" t="s">
+      <c r="B95" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="C95" s="65" t="s">
+      <c r="C95" s="39" t="s">
         <v>66</v>
       </c>
       <c r="F95" t="s">
@@ -26241,7 +26241,7 @@
       <c r="M95" t="s">
         <v>211</v>
       </c>
-      <c r="N95" s="71" t="s">
+      <c r="N95" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -26249,10 +26249,10 @@
       <c r="A96">
         <v>87</v>
       </c>
-      <c r="B96" s="65" t="s">
+      <c r="B96" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="C96" s="65" t="s">
+      <c r="C96" s="39" t="s">
         <v>66</v>
       </c>
       <c r="F96" t="s">
@@ -26273,7 +26273,7 @@
       <c r="M96" t="s">
         <v>211</v>
       </c>
-      <c r="N96" s="71" t="s">
+      <c r="N96" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -26281,10 +26281,10 @@
       <c r="A97">
         <v>88</v>
       </c>
-      <c r="B97" s="65" t="s">
+      <c r="B97" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="C97" s="65" t="s">
+      <c r="C97" s="39" t="s">
         <v>66</v>
       </c>
       <c r="F97" t="s">
@@ -26305,7 +26305,7 @@
       <c r="M97" t="s">
         <v>211</v>
       </c>
-      <c r="N97" s="71" t="s">
+      <c r="N97" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -26313,10 +26313,10 @@
       <c r="A98">
         <v>89</v>
       </c>
-      <c r="B98" s="65" t="s">
+      <c r="B98" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="C98" s="65" t="s">
+      <c r="C98" s="39" t="s">
         <v>66</v>
       </c>
       <c r="F98" t="s">
@@ -26337,7 +26337,7 @@
       <c r="M98" t="s">
         <v>211</v>
       </c>
-      <c r="N98" s="71" t="s">
+      <c r="N98" s="45" t="s">
         <v>219</v>
       </c>
     </row>
@@ -26345,10 +26345,10 @@
       <c r="A99">
         <v>90</v>
       </c>
-      <c r="B99" s="65" t="s">
+      <c r="B99" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="C99" s="65" t="s">
+      <c r="C99" s="39" t="s">
         <v>106</v>
       </c>
       <c r="F99" t="s">
@@ -26359,7 +26359,7 @@
       </c>
       <c r="H99" s="35"/>
       <c r="I99" s="37">
-        <v>35.709364908503602</v>
+        <v>298</v>
       </c>
       <c r="J99" s="34">
         <v>4938775523.3745441</v>
@@ -26369,7 +26369,7 @@
       <c r="M99" t="s">
         <v>220</v>
       </c>
-      <c r="N99" s="71" t="s">
+      <c r="N99" s="45" t="s">
         <v>221</v>
       </c>
     </row>
@@ -26377,10 +26377,10 @@
       <c r="A100">
         <v>91</v>
       </c>
-      <c r="B100" s="65" t="s">
+      <c r="B100" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="C100" s="65" t="s">
+      <c r="C100" s="39" t="s">
         <v>106</v>
       </c>
       <c r="F100" t="s">
@@ -26391,7 +26391,7 @@
       </c>
       <c r="H100" s="35"/>
       <c r="I100" s="37">
-        <v>289.43379978471398</v>
+        <v>473</v>
       </c>
       <c r="J100" s="34">
         <v>4559037054.7166595</v>
@@ -26401,7 +26401,7 @@
       <c r="M100" t="s">
         <v>220</v>
       </c>
-      <c r="N100" s="71" t="s">
+      <c r="N100" s="45" t="s">
         <v>221</v>
       </c>
     </row>
@@ -26409,10 +26409,10 @@
       <c r="A101">
         <v>92</v>
       </c>
-      <c r="B101" s="65" t="s">
+      <c r="B101" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="C101" s="65" t="s">
+      <c r="C101" s="39" t="s">
         <v>106</v>
       </c>
       <c r="F101" t="s">
@@ -26423,7 +26423,7 @@
       </c>
       <c r="H101" s="35"/>
       <c r="I101" s="37">
-        <v>580.747039827771</v>
+        <v>673</v>
       </c>
       <c r="J101" s="34">
         <v>3944188036.7041183</v>
@@ -26433,7 +26433,7 @@
       <c r="M101" t="s">
         <v>220</v>
       </c>
-      <c r="N101" s="71" t="s">
+      <c r="N101" s="45" t="s">
         <v>221</v>
       </c>
     </row>
@@ -26441,10 +26441,10 @@
       <c r="A102">
         <v>93</v>
       </c>
-      <c r="B102" s="65" t="s">
+      <c r="B102" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="C102" s="65" t="s">
+      <c r="C102" s="39" t="s">
         <v>106</v>
       </c>
       <c r="F102" t="s">
@@ -26455,7 +26455,7 @@
       </c>
       <c r="H102" s="35"/>
       <c r="I102" s="37">
-        <v>872.06027987082803</v>
+        <v>873</v>
       </c>
       <c r="J102" s="34">
         <v>3547017757.0093436</v>
@@ -26465,7 +26465,7 @@
       <c r="M102" t="s">
         <v>220</v>
       </c>
-      <c r="N102" s="71" t="s">
+      <c r="N102" s="45" t="s">
         <v>221</v>
       </c>
     </row>
@@ -26473,10 +26473,10 @@
       <c r="A103">
         <v>94</v>
       </c>
-      <c r="B103" s="65" t="s">
+      <c r="B103" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="C103" s="65" t="s">
+      <c r="C103" s="39" t="s">
         <v>106</v>
       </c>
       <c r="F103" t="s">
@@ -26487,7 +26487,7 @@
       </c>
       <c r="H103" s="35"/>
       <c r="I103" s="37">
-        <v>1164.31324004305</v>
+        <v>1073</v>
       </c>
       <c r="J103" s="34">
         <v>3304507783.0900407</v>
@@ -26497,7 +26497,7 @@
       <c r="M103" t="s">
         <v>220</v>
       </c>
-      <c r="N103" s="71" t="s">
+      <c r="N103" s="45" t="s">
         <v>221</v>
       </c>
     </row>
@@ -26505,10 +26505,10 @@
       <c r="A104">
         <v>95</v>
       </c>
-      <c r="B104" s="65" t="s">
+      <c r="B104" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="C104" s="65" t="s">
+      <c r="C104" s="39" t="s">
         <v>106</v>
       </c>
       <c r="F104" t="s">
@@ -26519,7 +26519,7 @@
       </c>
       <c r="H104" s="35"/>
       <c r="I104" s="37">
-        <v>1455.62648008611</v>
+        <v>1273</v>
       </c>
       <c r="J104" s="34">
         <v>3073460751.0588222</v>
@@ -26529,7 +26529,7 @@
       <c r="M104" t="s">
         <v>220</v>
       </c>
-      <c r="N104" s="71" t="s">
+      <c r="N104" s="45" t="s">
         <v>221</v>
       </c>
     </row>
@@ -26537,10 +26537,10 @@
       <c r="A105">
         <v>96</v>
       </c>
-      <c r="B105" s="65" t="s">
+      <c r="B105" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="C105" s="65" t="s">
+      <c r="C105" s="39" t="s">
         <v>106</v>
       </c>
       <c r="F105" t="s">
@@ -26551,7 +26551,7 @@
       </c>
       <c r="H105" s="35"/>
       <c r="I105" s="37">
-        <v>34.769644779332403</v>
+        <v>298</v>
       </c>
       <c r="J105" s="34">
         <v>6410977367.1317739</v>
@@ -26561,7 +26561,7 @@
       <c r="M105" t="s">
         <v>220</v>
       </c>
-      <c r="N105" s="71" t="s">
+      <c r="N105" s="45" t="s">
         <v>221</v>
       </c>
     </row>
@@ -26569,10 +26569,10 @@
       <c r="A106">
         <v>97</v>
       </c>
-      <c r="B106" s="65" t="s">
+      <c r="B106" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="C106" s="65" t="s">
+      <c r="C106" s="39" t="s">
         <v>106</v>
       </c>
       <c r="F106" t="s">
@@ -26583,7 +26583,7 @@
       </c>
       <c r="H106" s="35"/>
       <c r="I106" s="37">
-        <v>141.897739504843</v>
+        <v>373</v>
       </c>
       <c r="J106" s="34">
         <v>6083756314.3214979</v>
@@ -26593,7 +26593,7 @@
       <c r="M106" t="s">
         <v>220</v>
       </c>
-      <c r="N106" s="71" t="s">
+      <c r="N106" s="45" t="s">
         <v>221</v>
       </c>
     </row>
@@ -26601,10 +26601,10 @@
       <c r="A107">
         <v>98</v>
       </c>
-      <c r="B107" s="65" t="s">
+      <c r="B107" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="C107" s="65" t="s">
+      <c r="C107" s="39" t="s">
         <v>106</v>
       </c>
       <c r="F107" t="s">
@@ -26615,7 +26615,7 @@
       </c>
       <c r="H107" s="35"/>
       <c r="I107" s="37">
-        <v>288.49407965554298</v>
+        <v>473</v>
       </c>
       <c r="J107" s="34">
         <v>5836473711.5579948</v>
@@ -26625,7 +26625,7 @@
       <c r="M107" t="s">
         <v>220</v>
       </c>
-      <c r="N107" s="71" t="s">
+      <c r="N107" s="45" t="s">
         <v>221</v>
       </c>
     </row>
@@ -26633,10 +26633,10 @@
       <c r="A108">
         <v>99</v>
       </c>
-      <c r="B108" s="65" t="s">
+      <c r="B108" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="C108" s="65" t="s">
+      <c r="C108" s="39" t="s">
         <v>106</v>
       </c>
       <c r="F108" t="s">
@@ -26647,7 +26647,7 @@
       </c>
       <c r="H108" s="35"/>
       <c r="I108" s="37">
-        <v>434.15069967707097</v>
+        <v>573</v>
       </c>
       <c r="J108" s="34">
         <v>5520456620.7760334</v>
@@ -26657,7 +26657,7 @@
       <c r="M108" t="s">
         <v>220</v>
       </c>
-      <c r="N108" s="71" t="s">
+      <c r="N108" s="45" t="s">
         <v>221</v>
       </c>
     </row>
@@ -26665,10 +26665,10 @@
       <c r="A109">
         <v>100</v>
       </c>
-      <c r="B109" s="65" t="s">
+      <c r="B109" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="C109" s="65" t="s">
+      <c r="C109" s="39" t="s">
         <v>106</v>
       </c>
       <c r="F109" t="s">
@@ -26679,7 +26679,7 @@
       </c>
       <c r="H109" s="35"/>
       <c r="I109" s="37">
-        <v>579.80731969860005</v>
+        <v>673</v>
       </c>
       <c r="J109" s="34">
         <v>5336192450.5548067</v>
@@ -26689,7 +26689,7 @@
       <c r="M109" t="s">
         <v>220</v>
       </c>
-      <c r="N109" s="71" t="s">
+      <c r="N109" s="45" t="s">
         <v>221</v>
       </c>
     </row>
@@ -26697,10 +26697,10 @@
       <c r="A110">
         <v>101</v>
       </c>
-      <c r="B110" s="65" t="s">
+      <c r="B110" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="C110" s="65" t="s">
+      <c r="C110" s="39" t="s">
         <v>106</v>
       </c>
       <c r="F110" t="s">
@@ -26711,7 +26711,7 @@
       </c>
       <c r="H110" s="35"/>
       <c r="I110" s="37">
-        <v>728.28310010764199</v>
+        <v>773</v>
       </c>
       <c r="J110" s="34">
         <v>5071712351.8656368</v>
@@ -26721,7 +26721,7 @@
       <c r="M110" t="s">
         <v>220</v>
       </c>
-      <c r="N110" s="71" t="s">
+      <c r="N110" s="45" t="s">
         <v>221</v>
       </c>
     </row>
@@ -26729,10 +26729,10 @@
       <c r="A111">
         <v>102</v>
       </c>
-      <c r="B111" s="65" t="s">
+      <c r="B111" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="C111" s="65" t="s">
+      <c r="C111" s="39" t="s">
         <v>106</v>
       </c>
       <c r="F111" t="s">
@@ -26743,7 +26743,7 @@
       </c>
       <c r="H111" s="35"/>
       <c r="I111" s="37">
-        <v>872.99999999999898</v>
+        <v>873</v>
       </c>
       <c r="J111" s="34">
         <v>5139503413.2521124</v>
@@ -26753,7 +26753,7 @@
       <c r="M111" t="s">
         <v>220</v>
       </c>
-      <c r="N111" s="71" t="s">
+      <c r="N111" s="45" t="s">
         <v>221</v>
       </c>
     </row>
@@ -26761,10 +26761,10 @@
       <c r="A112">
         <v>103</v>
       </c>
-      <c r="B112" s="65" t="s">
+      <c r="B112" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="C112" s="65" t="s">
+      <c r="C112" s="39" t="s">
         <v>106</v>
       </c>
       <c r="F112" t="s">
@@ -26775,7 +26775,7 @@
       </c>
       <c r="H112" s="35"/>
       <c r="I112" s="37">
-        <v>1021.47578040904</v>
+        <v>973</v>
       </c>
       <c r="J112" s="34">
         <v>4915122029.5162029</v>
@@ -26785,7 +26785,7 @@
       <c r="M112" t="s">
         <v>220</v>
       </c>
-      <c r="N112" s="71" t="s">
+      <c r="N112" s="45" t="s">
         <v>221</v>
       </c>
     </row>
@@ -26793,10 +26793,10 @@
       <c r="A113">
         <v>104</v>
       </c>
-      <c r="B113" s="65" t="s">
+      <c r="B113" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="C113" s="65" t="s">
+      <c r="C113" s="39" t="s">
         <v>106</v>
       </c>
       <c r="F113" t="s">
@@ -26807,7 +26807,7 @@
       </c>
       <c r="H113" s="35"/>
       <c r="I113" s="37">
-        <v>1163.37351991388</v>
+        <v>1073</v>
       </c>
       <c r="J113" s="34">
         <v>4541845724.9781151</v>
@@ -26817,7 +26817,7 @@
       <c r="M113" t="s">
         <v>220</v>
       </c>
-      <c r="N113" s="71" t="s">
+      <c r="N113" s="45" t="s">
         <v>221</v>
       </c>
     </row>
@@ -26825,10 +26825,10 @@
       <c r="A114">
         <v>105</v>
       </c>
-      <c r="B114" s="65" t="s">
+      <c r="B114" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="C114" s="65" t="s">
+      <c r="C114" s="39" t="s">
         <v>106</v>
       </c>
       <c r="F114" t="s">
@@ -26839,7 +26839,7 @@
       </c>
       <c r="H114" s="35"/>
       <c r="I114" s="37">
-        <v>1309.03013993541</v>
+        <v>1173</v>
       </c>
       <c r="J114" s="34">
         <v>4644000947.2802582</v>
@@ -26849,7 +26849,7 @@
       <c r="M114" t="s">
         <v>220</v>
       </c>
-      <c r="N114" s="71" t="s">
+      <c r="N114" s="45" t="s">
         <v>221</v>
       </c>
     </row>
@@ -26857,10 +26857,10 @@
       <c r="A115">
         <v>106</v>
       </c>
-      <c r="B115" s="65" t="s">
+      <c r="B115" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="C115" s="65" t="s">
+      <c r="C115" s="39" t="s">
         <v>106</v>
       </c>
       <c r="F115" t="s">
@@ -26871,7 +26871,7 @@
       </c>
       <c r="H115" s="35"/>
       <c r="I115" s="37">
-        <v>1455.62648008611</v>
+        <v>1273</v>
       </c>
       <c r="J115" s="34">
         <v>4310792526.7597532</v>
@@ -26881,7 +26881,7 @@
       <c r="M115" t="s">
         <v>220</v>
       </c>
-      <c r="N115" s="71" t="s">
+      <c r="N115" s="45" t="s">
         <v>221</v>
       </c>
     </row>
@@ -26889,10 +26889,10 @@
       <c r="A116">
         <v>107</v>
       </c>
-      <c r="B116" s="65" t="s">
+      <c r="B116" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="C116" s="65" t="s">
+      <c r="C116" s="39" t="s">
         <v>106</v>
       </c>
       <c r="F116" t="s">
@@ -26903,7 +26903,7 @@
       </c>
       <c r="H116" s="35"/>
       <c r="I116" s="37">
-        <v>33.829924650161303</v>
+        <v>298</v>
       </c>
       <c r="J116" s="34">
         <v>7287426874.4404078</v>
@@ -26913,7 +26913,7 @@
       <c r="M116" t="s">
         <v>220</v>
       </c>
-      <c r="N116" s="71" t="s">
+      <c r="N116" s="45" t="s">
         <v>221</v>
       </c>
     </row>
@@ -26921,10 +26921,10 @@
       <c r="A117">
         <v>108</v>
       </c>
-      <c r="B117" s="65" t="s">
+      <c r="B117" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="C117" s="65" t="s">
+      <c r="C117" s="39" t="s">
         <v>106</v>
       </c>
       <c r="F117" t="s">
@@ -26935,7 +26935,7 @@
       </c>
       <c r="H117" s="35"/>
       <c r="I117" s="37">
-        <v>287.55435952637202</v>
+        <v>473</v>
       </c>
       <c r="J117" s="34">
         <v>6243195415.1283121</v>
@@ -26945,7 +26945,7 @@
       <c r="M117" t="s">
         <v>220</v>
       </c>
-      <c r="N117" s="71" t="s">
+      <c r="N117" s="45" t="s">
         <v>221</v>
       </c>
     </row>
@@ -26953,10 +26953,10 @@
       <c r="A118">
         <v>109</v>
       </c>
-      <c r="B118" s="65" t="s">
+      <c r="B118" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="C118" s="65" t="s">
+      <c r="C118" s="39" t="s">
         <v>106</v>
       </c>
       <c r="F118" t="s">
@@ -26967,7 +26967,7 @@
       </c>
       <c r="H118" s="35"/>
       <c r="I118" s="37">
-        <v>580.747039827771</v>
+        <v>673</v>
       </c>
       <c r="J118" s="34">
         <v>5828827639.5078602</v>
@@ -26977,7 +26977,7 @@
       <c r="M118" t="s">
         <v>220</v>
       </c>
-      <c r="N118" s="71" t="s">
+      <c r="N118" s="45" t="s">
         <v>221</v>
       </c>
     </row>
@@ -26985,10 +26985,10 @@
       <c r="A119">
         <v>110</v>
       </c>
-      <c r="B119" s="65" t="s">
+      <c r="B119" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="C119" s="65" t="s">
+      <c r="C119" s="39" t="s">
         <v>106</v>
       </c>
       <c r="F119" t="s">
@@ -26999,7 +26999,7 @@
       </c>
       <c r="H119" s="35"/>
       <c r="I119" s="37">
-        <v>872.99999999999898</v>
+        <v>873</v>
       </c>
       <c r="J119" s="34">
         <v>5351453763.7193985</v>
@@ -27009,7 +27009,7 @@
       <c r="M119" t="s">
         <v>220</v>
       </c>
-      <c r="N119" s="71" t="s">
+      <c r="N119" s="45" t="s">
         <v>221</v>
       </c>
     </row>
@@ -27017,10 +27017,10 @@
       <c r="A120">
         <v>111</v>
       </c>
-      <c r="B120" s="65" t="s">
+      <c r="B120" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="C120" s="65" t="s">
+      <c r="C120" s="39" t="s">
         <v>106</v>
       </c>
       <c r="F120" t="s">
@@ -27031,7 +27031,7 @@
       </c>
       <c r="H120" s="35"/>
       <c r="I120" s="37">
-        <v>1163.37351991388</v>
+        <v>1073</v>
       </c>
       <c r="J120" s="34">
         <v>5091770958.6229734</v>
@@ -27041,7 +27041,7 @@
       <c r="M120" t="s">
         <v>220</v>
       </c>
-      <c r="N120" s="71" t="s">
+      <c r="N120" s="45" t="s">
         <v>221</v>
       </c>
     </row>
@@ -27049,10 +27049,10 @@
       <c r="A121">
         <v>112</v>
       </c>
-      <c r="B121" s="65" t="s">
+      <c r="B121" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="C121" s="65" t="s">
+      <c r="C121" s="39" t="s">
         <v>106</v>
       </c>
       <c r="F121" t="s">
@@ -27063,7 +27063,7 @@
       </c>
       <c r="H121" s="35"/>
       <c r="I121" s="37">
-        <v>1454.68675995694</v>
+        <v>1273</v>
       </c>
       <c r="J121" s="34">
         <v>4648773576.1244574</v>
@@ -27073,7 +27073,7 @@
       <c r="M121" t="s">
         <v>220</v>
       </c>
-      <c r="N121" s="71" t="s">
+      <c r="N121" s="45" t="s">
         <v>221</v>
       </c>
     </row>
@@ -27081,16 +27081,16 @@
       <c r="A122">
         <v>113</v>
       </c>
-      <c r="B122" s="65" t="s">
+      <c r="B122" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="C122" s="65" t="s">
+      <c r="C122" s="39" t="s">
         <v>105</v>
       </c>
       <c r="D122" t="s">
         <v>92</v>
       </c>
-      <c r="E122" s="68" t="s">
+      <c r="E122" s="42" t="s">
         <v>102</v>
       </c>
       <c r="F122" t="s">
@@ -27111,7 +27111,7 @@
       <c r="M122" t="s">
         <v>222</v>
       </c>
-      <c r="N122" s="71" t="s">
+      <c r="N122" s="45" t="s">
         <v>223</v>
       </c>
     </row>
@@ -27119,16 +27119,16 @@
       <c r="A123">
         <v>114</v>
       </c>
-      <c r="B123" s="65" t="s">
+      <c r="B123" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="C123" s="65" t="s">
+      <c r="C123" s="39" t="s">
         <v>66</v>
       </c>
       <c r="D123" t="s">
         <v>92</v>
       </c>
-      <c r="E123" s="68" t="s">
+      <c r="E123" s="42" t="s">
         <v>101</v>
       </c>
       <c r="F123" t="s">
@@ -27149,7 +27149,7 @@
       <c r="M123" t="s">
         <v>222</v>
       </c>
-      <c r="N123" s="71" t="s">
+      <c r="N123" s="45" t="s">
         <v>223</v>
       </c>
     </row>
@@ -27157,16 +27157,16 @@
       <c r="A124">
         <v>115</v>
       </c>
-      <c r="B124" s="65" t="s">
+      <c r="B124" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="C124" s="65" t="s">
+      <c r="C124" s="39" t="s">
         <v>66</v>
       </c>
       <c r="D124" t="s">
         <v>92</v>
       </c>
-      <c r="E124" s="68" t="s">
+      <c r="E124" s="42" t="s">
         <v>100</v>
       </c>
       <c r="F124" t="s">
@@ -27187,7 +27187,7 @@
       <c r="M124" t="s">
         <v>222</v>
       </c>
-      <c r="N124" s="71" t="s">
+      <c r="N124" s="45" t="s">
         <v>223</v>
       </c>
     </row>
@@ -27195,16 +27195,16 @@
       <c r="A125">
         <v>116</v>
       </c>
-      <c r="B125" s="65" t="s">
+      <c r="B125" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="C125" s="65" t="s">
+      <c r="C125" s="39" t="s">
         <v>66</v>
       </c>
       <c r="D125" t="s">
         <v>92</v>
       </c>
-      <c r="E125" s="68" t="s">
+      <c r="E125" s="42" t="s">
         <v>99</v>
       </c>
       <c r="F125" t="s">
@@ -27225,7 +27225,7 @@
       <c r="M125" t="s">
         <v>222</v>
       </c>
-      <c r="N125" s="71" t="s">
+      <c r="N125" s="45" t="s">
         <v>223</v>
       </c>
     </row>
@@ -27233,16 +27233,16 @@
       <c r="A126">
         <v>117</v>
       </c>
-      <c r="B126" s="65" t="s">
+      <c r="B126" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="C126" s="65" t="s">
+      <c r="C126" s="39" t="s">
         <v>103</v>
       </c>
       <c r="D126" t="s">
         <v>92</v>
       </c>
-      <c r="E126" s="68" t="s">
+      <c r="E126" s="42" t="s">
         <v>96</v>
       </c>
       <c r="F126" t="s">
@@ -27263,7 +27263,7 @@
       <c r="M126" t="s">
         <v>222</v>
       </c>
-      <c r="N126" s="71" t="s">
+      <c r="N126" s="45" t="s">
         <v>223</v>
       </c>
     </row>
@@ -27271,16 +27271,16 @@
       <c r="A127">
         <v>118</v>
       </c>
-      <c r="B127" s="65" t="s">
+      <c r="B127" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="C127" s="65" t="s">
+      <c r="C127" s="39" t="s">
         <v>97</v>
       </c>
       <c r="D127" t="s">
         <v>92</v>
       </c>
-      <c r="E127" s="68" t="s">
+      <c r="E127" s="42" t="s">
         <v>102</v>
       </c>
       <c r="F127" t="s">
@@ -27301,7 +27301,7 @@
       <c r="M127" t="s">
         <v>222</v>
       </c>
-      <c r="N127" s="71" t="s">
+      <c r="N127" s="45" t="s">
         <v>223</v>
       </c>
     </row>
@@ -27309,16 +27309,16 @@
       <c r="A128">
         <v>119</v>
       </c>
-      <c r="B128" s="65" t="s">
+      <c r="B128" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="C128" s="65" t="s">
+      <c r="C128" s="39" t="s">
         <v>97</v>
       </c>
       <c r="D128" t="s">
         <v>92</v>
       </c>
-      <c r="E128" s="68" t="s">
+      <c r="E128" s="42" t="s">
         <v>101</v>
       </c>
       <c r="F128" t="s">
@@ -27339,7 +27339,7 @@
       <c r="M128" t="s">
         <v>222</v>
       </c>
-      <c r="N128" s="71" t="s">
+      <c r="N128" s="45" t="s">
         <v>223</v>
       </c>
     </row>
@@ -27347,16 +27347,16 @@
       <c r="A129">
         <v>120</v>
       </c>
-      <c r="B129" s="65" t="s">
+      <c r="B129" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="C129" s="65" t="s">
+      <c r="C129" s="39" t="s">
         <v>97</v>
       </c>
       <c r="D129" t="s">
         <v>92</v>
       </c>
-      <c r="E129" s="68" t="s">
+      <c r="E129" s="42" t="s">
         <v>100</v>
       </c>
       <c r="F129" t="s">
@@ -27377,7 +27377,7 @@
       <c r="M129" t="s">
         <v>222</v>
       </c>
-      <c r="N129" s="71" t="s">
+      <c r="N129" s="45" t="s">
         <v>223</v>
       </c>
     </row>
@@ -27385,16 +27385,16 @@
       <c r="A130">
         <v>121</v>
       </c>
-      <c r="B130" s="65" t="s">
+      <c r="B130" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="C130" s="65" t="s">
+      <c r="C130" s="39" t="s">
         <v>97</v>
       </c>
       <c r="D130" t="s">
         <v>92</v>
       </c>
-      <c r="E130" s="68" t="s">
+      <c r="E130" s="42" t="s">
         <v>99</v>
       </c>
       <c r="F130" t="s">
@@ -27415,7 +27415,7 @@
       <c r="M130" t="s">
         <v>222</v>
       </c>
-      <c r="N130" s="71" t="s">
+      <c r="N130" s="45" t="s">
         <v>223</v>
       </c>
     </row>
@@ -27423,16 +27423,16 @@
       <c r="A131">
         <v>122</v>
       </c>
-      <c r="B131" s="65" t="s">
+      <c r="B131" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="C131" s="65" t="s">
+      <c r="C131" s="39" t="s">
         <v>97</v>
       </c>
       <c r="D131" t="s">
         <v>92</v>
       </c>
-      <c r="E131" s="68" t="s">
+      <c r="E131" s="42" t="s">
         <v>96</v>
       </c>
       <c r="F131" t="s">
@@ -27453,7 +27453,7 @@
       <c r="M131" t="s">
         <v>222</v>
       </c>
-      <c r="N131" s="71" t="s">
+      <c r="N131" s="45" t="s">
         <v>223</v>
       </c>
     </row>
@@ -27461,16 +27461,16 @@
       <c r="A132">
         <v>123</v>
       </c>
-      <c r="B132" s="65" t="s">
+      <c r="B132" s="39" t="s">
         <v>95</v>
       </c>
-      <c r="C132" s="65" t="s">
+      <c r="C132" s="39" t="s">
         <v>66</v>
       </c>
       <c r="D132" t="s">
         <v>92</v>
       </c>
-      <c r="E132" s="68" t="s">
+      <c r="E132" s="42" t="s">
         <v>91</v>
       </c>
       <c r="F132" t="s">
@@ -27491,7 +27491,7 @@
       <c r="M132" t="s">
         <v>222</v>
       </c>
-      <c r="N132" s="71" t="s">
+      <c r="N132" s="45" t="s">
         <v>223</v>
       </c>
     </row>
@@ -27499,16 +27499,16 @@
       <c r="A133">
         <v>124</v>
       </c>
-      <c r="B133" s="65" t="s">
+      <c r="B133" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="C133" s="65" t="s">
+      <c r="C133" s="39" t="s">
         <v>66</v>
       </c>
       <c r="D133" t="s">
         <v>92</v>
       </c>
-      <c r="E133" s="68" t="s">
+      <c r="E133" s="42" t="s">
         <v>91</v>
       </c>
       <c r="F133" t="s">
@@ -27529,7 +27529,7 @@
       <c r="M133" t="s">
         <v>222</v>
       </c>
-      <c r="N133" s="71" t="s">
+      <c r="N133" s="45" t="s">
         <v>223</v>
       </c>
     </row>
@@ -27537,16 +27537,16 @@
       <c r="A134">
         <v>125</v>
       </c>
-      <c r="B134" s="65" t="s">
+      <c r="B134" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="C134" s="65" t="s">
+      <c r="C134" s="39" t="s">
         <v>66</v>
       </c>
       <c r="D134" t="s">
         <v>92</v>
       </c>
-      <c r="E134" s="68" t="s">
+      <c r="E134" s="42" t="s">
         <v>91</v>
       </c>
       <c r="F134" t="s">
@@ -27567,7 +27567,7 @@
       <c r="M134" t="s">
         <v>222</v>
       </c>
-      <c r="N134" s="71" t="s">
+      <c r="N134" s="45" t="s">
         <v>223</v>
       </c>
     </row>
@@ -27575,10 +27575,10 @@
       <c r="A135">
         <v>126</v>
       </c>
-      <c r="B135" s="65" t="s">
+      <c r="B135" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="C135" s="65" t="s">
+      <c r="C135" s="39" t="s">
         <v>84</v>
       </c>
       <c r="F135" t="s">
@@ -27599,7 +27599,7 @@
       <c r="M135" t="s">
         <v>224</v>
       </c>
-      <c r="N135" s="72" t="s">
+      <c r="N135" s="46" t="s">
         <v>225</v>
       </c>
     </row>
@@ -27607,10 +27607,10 @@
       <c r="A136">
         <v>127</v>
       </c>
-      <c r="B136" s="65" t="s">
+      <c r="B136" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="C136" s="65" t="s">
+      <c r="C136" s="39" t="s">
         <v>66</v>
       </c>
       <c r="F136" t="s">
@@ -27631,7 +27631,7 @@
       <c r="M136" t="s">
         <v>224</v>
       </c>
-      <c r="N136" s="72" t="s">
+      <c r="N136" s="46" t="s">
         <v>225</v>
       </c>
     </row>
@@ -27639,10 +27639,10 @@
       <c r="A137">
         <v>128</v>
       </c>
-      <c r="B137" s="65" t="s">
+      <c r="B137" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="C137" s="65" t="s">
+      <c r="C137" s="39" t="s">
         <v>66</v>
       </c>
       <c r="F137" t="s">
@@ -27663,7 +27663,7 @@
       <c r="M137" t="s">
         <v>224</v>
       </c>
-      <c r="N137" s="72" t="s">
+      <c r="N137" s="46" t="s">
         <v>225</v>
       </c>
     </row>
@@ -27671,10 +27671,10 @@
       <c r="A138">
         <v>129</v>
       </c>
-      <c r="B138" s="65" t="s">
+      <c r="B138" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="C138" s="65" t="s">
+      <c r="C138" s="39" t="s">
         <v>84</v>
       </c>
       <c r="F138" t="s">
@@ -27695,7 +27695,7 @@
       <c r="M138" t="s">
         <v>224</v>
       </c>
-      <c r="N138" s="72" t="s">
+      <c r="N138" s="46" t="s">
         <v>225</v>
       </c>
     </row>
@@ -27703,10 +27703,10 @@
       <c r="A139">
         <v>130</v>
       </c>
-      <c r="B139" s="65" t="s">
+      <c r="B139" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="C139" s="65" t="s">
+      <c r="C139" s="39" t="s">
         <v>66</v>
       </c>
       <c r="F139" t="s">
@@ -27727,7 +27727,7 @@
       <c r="M139" t="s">
         <v>224</v>
       </c>
-      <c r="N139" s="72" t="s">
+      <c r="N139" s="46" t="s">
         <v>225</v>
       </c>
     </row>
@@ -27735,10 +27735,10 @@
       <c r="A140">
         <v>131</v>
       </c>
-      <c r="B140" s="65" t="s">
+      <c r="B140" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="C140" s="65" t="s">
+      <c r="C140" s="39" t="s">
         <v>84</v>
       </c>
       <c r="F140" t="s">
@@ -27759,7 +27759,7 @@
       <c r="M140" t="s">
         <v>224</v>
       </c>
-      <c r="N140" s="72" t="s">
+      <c r="N140" s="46" t="s">
         <v>225</v>
       </c>
     </row>
@@ -27767,10 +27767,10 @@
       <c r="A141">
         <v>132</v>
       </c>
-      <c r="B141" s="65" t="s">
+      <c r="B141" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="C141" s="65" t="s">
+      <c r="C141" s="39" t="s">
         <v>61</v>
       </c>
       <c r="F141" t="s">
@@ -27791,7 +27791,7 @@
       <c r="M141" t="s">
         <v>226</v>
       </c>
-      <c r="N141" s="71" t="s">
+      <c r="N141" s="45" t="s">
         <v>227</v>
       </c>
     </row>
@@ -27799,10 +27799,10 @@
       <c r="A142">
         <v>133</v>
       </c>
-      <c r="B142" s="65" t="s">
+      <c r="B142" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="C142" s="65" t="s">
+      <c r="C142" s="39" t="s">
         <v>81</v>
       </c>
       <c r="D142" t="s">
@@ -27834,10 +27834,10 @@
       <c r="A143">
         <v>134</v>
       </c>
-      <c r="B143" s="67" t="s">
+      <c r="B143" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="C143" s="67" t="s">
+      <c r="C143" s="41" t="s">
         <v>78</v>
       </c>
       <c r="D143" t="s">
@@ -27869,10 +27869,10 @@
       <c r="A144">
         <v>135</v>
       </c>
-      <c r="B144" s="66" t="s">
+      <c r="B144" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="C144" s="65" t="s">
+      <c r="C144" s="39" t="s">
         <v>75</v>
       </c>
       <c r="F144" t="s">
@@ -27893,7 +27893,7 @@
       <c r="M144" t="s">
         <v>222</v>
       </c>
-      <c r="N144" s="71" t="s">
+      <c r="N144" s="45" t="s">
         <v>230</v>
       </c>
     </row>
@@ -27901,10 +27901,10 @@
       <c r="A145">
         <v>136</v>
       </c>
-      <c r="B145" s="66" t="s">
+      <c r="B145" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C145" s="65" t="s">
+      <c r="C145" s="39" t="s">
         <v>66</v>
       </c>
       <c r="F145" t="s">
@@ -27925,7 +27925,7 @@
       <c r="M145" t="s">
         <v>222</v>
       </c>
-      <c r="N145" s="71" t="s">
+      <c r="N145" s="45" t="s">
         <v>230</v>
       </c>
     </row>
@@ -27936,7 +27936,7 @@
       <c r="B146" t="s">
         <v>73</v>
       </c>
-      <c r="C146" s="65" t="s">
+      <c r="C146" s="39" t="s">
         <v>71</v>
       </c>
       <c r="F146" t="s">
@@ -27968,7 +27968,7 @@
       <c r="B147" t="s">
         <v>72</v>
       </c>
-      <c r="C147" s="65" t="s">
+      <c r="C147" s="39" t="s">
         <v>71</v>
       </c>
       <c r="F147" t="s">
@@ -28000,7 +28000,7 @@
       <c r="B148" t="s">
         <v>70</v>
       </c>
-      <c r="C148" s="65" t="s">
+      <c r="C148" s="39" t="s">
         <v>68</v>
       </c>
       <c r="F148" t="s">
@@ -28032,7 +28032,7 @@
       <c r="B149" t="s">
         <v>69</v>
       </c>
-      <c r="C149" s="65" t="s">
+      <c r="C149" s="39" t="s">
         <v>68</v>
       </c>
       <c r="F149" t="s">
@@ -28085,7 +28085,7 @@
       <c r="M150" t="s">
         <v>211</v>
       </c>
-      <c r="N150" s="71" t="s">
+      <c r="N150" s="45" t="s">
         <v>233</v>
       </c>
     </row>
@@ -28117,7 +28117,7 @@
       <c r="M151" t="s">
         <v>211</v>
       </c>
-      <c r="N151" s="71" t="s">
+      <c r="N151" s="45" t="s">
         <v>233</v>
       </c>
     </row>
@@ -28149,7 +28149,7 @@
       <c r="M152" t="s">
         <v>211</v>
       </c>
-      <c r="N152" s="71" t="s">
+      <c r="N152" s="45" t="s">
         <v>233</v>
       </c>
     </row>
@@ -28181,7 +28181,7 @@
       <c r="M153" t="s">
         <v>211</v>
       </c>
-      <c r="N153" s="71" t="s">
+      <c r="N153" s="45" t="s">
         <v>233</v>
       </c>
     </row>
@@ -32150,6 +32150,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="P8:T8"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="H5:H6"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="B8:E8"/>
@@ -32164,11 +32169,6 @@
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="L5:L6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="P8:T8"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="H5:H6"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
- added processing history to `10.1016/j.intermet.2014.07.021`
</commit_message>
<xml_diff>
--- a/HuiSun_HardnessData_Jan2022_AdamFix.xlsx
+++ b/HuiSun_HardnessData_Jan2022_AdamFix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-guest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384F033E-A8A6-A541-983A-AF1000236E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A539637-58CC-1540-8E20-09D9E54B31BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="239">
   <si>
     <t>Name:</t>
   </si>
@@ -871,6 +871,12 @@
   </si>
   <si>
     <t>suh960@psu.edu</t>
+  </si>
+  <si>
+    <t>AAM+H+AT</t>
+  </si>
+  <si>
+    <t>homogenized at 1900*C for 1h followed by aging at 1300*C for 72h</t>
   </si>
 </sst>
 </file>
@@ -23099,8 +23105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="89" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F97" sqref="F97"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="89" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G107" sqref="G107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -26351,6 +26357,12 @@
       <c r="C99" s="39" t="s">
         <v>106</v>
       </c>
+      <c r="D99" t="s">
+        <v>237</v>
+      </c>
+      <c r="E99" t="s">
+        <v>238</v>
+      </c>
       <c r="F99" t="s">
         <v>204</v>
       </c>
@@ -26383,6 +26395,12 @@
       <c r="C100" s="39" t="s">
         <v>106</v>
       </c>
+      <c r="D100" t="s">
+        <v>237</v>
+      </c>
+      <c r="E100" t="s">
+        <v>238</v>
+      </c>
       <c r="F100" t="s">
         <v>204</v>
       </c>
@@ -26415,6 +26433,12 @@
       <c r="C101" s="39" t="s">
         <v>106</v>
       </c>
+      <c r="D101" t="s">
+        <v>237</v>
+      </c>
+      <c r="E101" t="s">
+        <v>238</v>
+      </c>
       <c r="F101" t="s">
         <v>204</v>
       </c>
@@ -26447,6 +26471,12 @@
       <c r="C102" s="39" t="s">
         <v>106</v>
       </c>
+      <c r="D102" t="s">
+        <v>237</v>
+      </c>
+      <c r="E102" t="s">
+        <v>238</v>
+      </c>
       <c r="F102" t="s">
         <v>204</v>
       </c>
@@ -26479,6 +26509,12 @@
       <c r="C103" s="39" t="s">
         <v>106</v>
       </c>
+      <c r="D103" t="s">
+        <v>237</v>
+      </c>
+      <c r="E103" t="s">
+        <v>238</v>
+      </c>
       <c r="F103" t="s">
         <v>204</v>
       </c>
@@ -26511,6 +26547,12 @@
       <c r="C104" s="39" t="s">
         <v>106</v>
       </c>
+      <c r="D104" t="s">
+        <v>237</v>
+      </c>
+      <c r="E104" t="s">
+        <v>238</v>
+      </c>
       <c r="F104" t="s">
         <v>204</v>
       </c>
@@ -26543,6 +26585,12 @@
       <c r="C105" s="39" t="s">
         <v>106</v>
       </c>
+      <c r="D105" t="s">
+        <v>237</v>
+      </c>
+      <c r="E105" t="s">
+        <v>238</v>
+      </c>
       <c r="F105" t="s">
         <v>204</v>
       </c>
@@ -26575,6 +26623,12 @@
       <c r="C106" s="39" t="s">
         <v>106</v>
       </c>
+      <c r="D106" t="s">
+        <v>237</v>
+      </c>
+      <c r="E106" t="s">
+        <v>238</v>
+      </c>
       <c r="F106" t="s">
         <v>204</v>
       </c>
@@ -26607,6 +26661,12 @@
       <c r="C107" s="39" t="s">
         <v>106</v>
       </c>
+      <c r="D107" t="s">
+        <v>237</v>
+      </c>
+      <c r="E107" t="s">
+        <v>238</v>
+      </c>
       <c r="F107" t="s">
         <v>204</v>
       </c>
@@ -26639,6 +26699,12 @@
       <c r="C108" s="39" t="s">
         <v>106</v>
       </c>
+      <c r="D108" t="s">
+        <v>237</v>
+      </c>
+      <c r="E108" t="s">
+        <v>238</v>
+      </c>
       <c r="F108" t="s">
         <v>204</v>
       </c>
@@ -26671,6 +26737,12 @@
       <c r="C109" s="39" t="s">
         <v>106</v>
       </c>
+      <c r="D109" t="s">
+        <v>237</v>
+      </c>
+      <c r="E109" t="s">
+        <v>238</v>
+      </c>
       <c r="F109" t="s">
         <v>204</v>
       </c>
@@ -26703,6 +26775,12 @@
       <c r="C110" s="39" t="s">
         <v>106</v>
       </c>
+      <c r="D110" t="s">
+        <v>237</v>
+      </c>
+      <c r="E110" t="s">
+        <v>238</v>
+      </c>
       <c r="F110" t="s">
         <v>204</v>
       </c>
@@ -26735,6 +26813,12 @@
       <c r="C111" s="39" t="s">
         <v>106</v>
       </c>
+      <c r="D111" t="s">
+        <v>237</v>
+      </c>
+      <c r="E111" t="s">
+        <v>238</v>
+      </c>
       <c r="F111" t="s">
         <v>204</v>
       </c>
@@ -26767,6 +26851,12 @@
       <c r="C112" s="39" t="s">
         <v>106</v>
       </c>
+      <c r="D112" t="s">
+        <v>237</v>
+      </c>
+      <c r="E112" t="s">
+        <v>238</v>
+      </c>
       <c r="F112" t="s">
         <v>204</v>
       </c>
@@ -26799,6 +26889,12 @@
       <c r="C113" s="39" t="s">
         <v>106</v>
       </c>
+      <c r="D113" t="s">
+        <v>237</v>
+      </c>
+      <c r="E113" t="s">
+        <v>238</v>
+      </c>
       <c r="F113" t="s">
         <v>204</v>
       </c>
@@ -26831,6 +26927,12 @@
       <c r="C114" s="39" t="s">
         <v>106</v>
       </c>
+      <c r="D114" t="s">
+        <v>237</v>
+      </c>
+      <c r="E114" t="s">
+        <v>238</v>
+      </c>
       <c r="F114" t="s">
         <v>204</v>
       </c>
@@ -26863,6 +26965,12 @@
       <c r="C115" s="39" t="s">
         <v>106</v>
       </c>
+      <c r="D115" t="s">
+        <v>237</v>
+      </c>
+      <c r="E115" t="s">
+        <v>238</v>
+      </c>
       <c r="F115" t="s">
         <v>204</v>
       </c>
@@ -26895,6 +27003,12 @@
       <c r="C116" s="39" t="s">
         <v>106</v>
       </c>
+      <c r="D116" t="s">
+        <v>237</v>
+      </c>
+      <c r="E116" t="s">
+        <v>238</v>
+      </c>
       <c r="F116" t="s">
         <v>204</v>
       </c>
@@ -26927,6 +27041,12 @@
       <c r="C117" s="39" t="s">
         <v>106</v>
       </c>
+      <c r="D117" t="s">
+        <v>237</v>
+      </c>
+      <c r="E117" t="s">
+        <v>238</v>
+      </c>
       <c r="F117" t="s">
         <v>204</v>
       </c>
@@ -26959,6 +27079,12 @@
       <c r="C118" s="39" t="s">
         <v>106</v>
       </c>
+      <c r="D118" t="s">
+        <v>237</v>
+      </c>
+      <c r="E118" t="s">
+        <v>238</v>
+      </c>
       <c r="F118" t="s">
         <v>204</v>
       </c>
@@ -26991,6 +27117,12 @@
       <c r="C119" s="39" t="s">
         <v>106</v>
       </c>
+      <c r="D119" t="s">
+        <v>237</v>
+      </c>
+      <c r="E119" t="s">
+        <v>238</v>
+      </c>
       <c r="F119" t="s">
         <v>204</v>
       </c>
@@ -27023,6 +27155,12 @@
       <c r="C120" s="39" t="s">
         <v>106</v>
       </c>
+      <c r="D120" t="s">
+        <v>237</v>
+      </c>
+      <c r="E120" t="s">
+        <v>238</v>
+      </c>
       <c r="F120" t="s">
         <v>204</v>
       </c>
@@ -27054,6 +27192,12 @@
       </c>
       <c r="C121" s="39" t="s">
         <v>106</v>
+      </c>
+      <c r="D121" t="s">
+        <v>237</v>
+      </c>
+      <c r="E121" t="s">
+        <v>238</v>
       </c>
       <c r="F121" t="s">
         <v>204</v>

</xml_diff>